<commit_message>
QuestionBoard -> Inquiry 로 수정
</commit_message>
<xml_diff>
--- a/프로젝트 산출물/5. 테이블명세서/Puppy Playtime 테이블 명세서.xlsx
+++ b/프로젝트 산출물/5. 테이블명세서/Puppy Playtime 테이블 명세서.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.4575"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="6690"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="10485"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="시트1" sheetId="1" r:id="rId4"/>
@@ -15,151 +15,343 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="128">
   <x:si>
+    <x:t>m_pw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 아이디</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_birth</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전화번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>s_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Null허용</x:t>
+  </x:si>
+  <x:si>
+    <x:t>생년월일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DATE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용현황</x:t>
+  </x:si>
+  <x:si>
+    <x:t>s_no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서비스명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필수약관1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록내용</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이메일주소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>데이터 타입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_num</x:t>
+  </x:si>
+  <x:si>
+    <x:t>케이지 번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_kind</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>승인여부</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>q_title</x:t>
+  </x:si>
+  <x:si>
+    <x:t>신청날짜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>r_no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>댓글번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_phone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필수약관2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>n_title</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NUMBER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>선택약관</x:t>
+  </x:si>
+  <x:si>
+    <x:t>케이지번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>n_no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서비스 번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>q_no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력값 F(female), M(male)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력값 small, middle, big</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 (Reservation_tbl)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개별 케이지 룸 (CageRoom_tbl)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부가서비스(ExtraService_tbl)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>문의 게시판 (Inquiry_tbl)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>견종</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>아이디</x:t>
+  </x:si>
+  <x:si>
+    <x:t>칼럼명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상태</x:t>
+  </x:si>
+  <x:si>
+    <x:t>N</x:t>
+  </x:si>
+  <x:si>
+    <x:t>펫번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>글번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>제목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유일키</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가격</x:t>
+  </x:si>
+  <x:si>
+    <x:t>체중</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사진</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유형</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>번호</x:t>
+  </x:si>
+  <x:si>
+    <x:t>크기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록자</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Y</x:t>
+  </x:si>
+  <x:si>
+    <x:t>키</x:t>
+  </x:si>
+  <x:si>
+    <x:t>한글명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>종류</x:t>
+  </x:si>
+  <x:si>
     <x:t>실제 예약 시작날짜</x:t>
   </x:si>
   <x:si>
-    <x:t>데이터 타입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>승인여부</x:t>
-  </x:si>
-  <x:si>
-    <x:t>p_num</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용현황</x:t>
-  </x:si>
-  <x:si>
-    <x:t>케이지 번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_kind</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_type</x:t>
-  </x:si>
-  <x:si>
-    <x:t>p_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>생년월일</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_pw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 아이디</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필수약관1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_birth</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전화번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_email</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등록내용</x:t>
-  </x:si>
-  <x:si>
-    <x:t>s_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Null허용</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이메일주소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>s_no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서비스명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>신청날짜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_phone</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필수약관2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>n_title</x:t>
-  </x:si>
-  <x:si>
-    <x:t>선택약관</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NUMBER</x:t>
-  </x:si>
-  <x:si>
-    <x:t>q_no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>q_title</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>r_no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>댓글번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>케이지번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>n_no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서비스 번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서비스 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결제가격</x:t>
-  </x:si>
-  <x:si>
-    <x:t>강아지사진</x:t>
-  </x:si>
-  <x:si>
-    <x:t>s_price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등록일시</x:t>
-  </x:si>
-  <x:si>
-    <x:t>테이블 명세서</x:t>
-  </x:si>
-  <x:si>
-    <x:t>특이사항</x:t>
+    <x:t>m_address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>reply_no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이미지 파일 경로명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_gender</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_required1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>r_startdate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_picture</x:t>
+  </x:si>
+  <x:si>
+    <x:t>r_approval</x:t>
+  </x:si>
+  <x:si>
+    <x:t>reply_title</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_usestatus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_explain</x:t>
+  </x:si>
+  <x:si>
+    <x:t>펫 (Pet_tbl)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>q_content</x:t>
+  </x:si>
+  <x:si>
+    <x:t>admin 고정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_required2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_picture</x:t>
+  </x:si>
+  <x:si>
+    <x:t>s_status</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_unique</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_dogbreed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>r_status</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c_status</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_weight</x:t>
+  </x:si>
+  <x:si>
+    <x:t>q_regdate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m_optional</x:t>
+  </x:si>
+  <x:si>
+    <x:t>n_content</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VARCHAR2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>s_explain</x:t>
+  </x:si>
+  <x:si>
+    <x:t>n_regdate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>r_payprice</x:t>
+  </x:si>
+  <x:si>
+    <x:t>r_enddate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>실제 예약 종료날짜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력값 using, reserved, unusing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공지사항 (Notice_TBL)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>reply_registrant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력값 Y(yes), N(no)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>특수문자 없이 숫자로만 구성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>reply_content</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력값 YYYY-MM-DD</x:t>
   </x:si>
   <x:si>
     <x:t>n_registrant</x:t>
@@ -169,235 +361,43 @@
   </x:si>
   <x:si>
     <x:t>댓글(Reply_tbl)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>특수문자 없이 숫자로만 구성</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">입력값 YYYY-MM-DD
 </x:t>
   </x:si>
   <x:si>
+    <x:t>회원 (Member_TBL)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력값 unuse, use</x:t>
+  </x:si>
+  <x:si>
     <x:t>reply_regdate</x:t>
   </x:si>
   <x:si>
-    <x:t>회원 (Member_TBL)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>입력값 YYYY-MM-DD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>reply_content</x:t>
-  </x:si>
-  <x:si>
     <x:t>8자리 이상 15자리 이내</x:t>
   </x:si>
   <x:si>
-    <x:t>입력값 F(female), M(male)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개별 케이지 룸 (CageRoom_tbl)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가서비스(ExtraService_tbl)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>입력값 small, middle, big</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 (Reservation_tbl)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>종류</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가격</x:t>
-  </x:si>
-  <x:si>
-    <x:t>N</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유형</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Y</x:t>
-  </x:si>
-  <x:si>
-    <x:t>키</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사진</x:t>
-  </x:si>
-  <x:si>
-    <x:t>견종</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>아이디</x:t>
-  </x:si>
-  <x:si>
-    <x:t>크기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>한글명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>칼럼명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>펫번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>글번호</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상태</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유일키</x:t>
-  </x:si>
-  <x:si>
-    <x:t>제목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>체중</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등록자</x:t>
-  </x:si>
-  <x:si>
-    <x:t>r_startdate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_picture</x:t>
-  </x:si>
-  <x:si>
-    <x:t>입력값 using, reserved, unusing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_address</x:t>
-  </x:si>
-  <x:si>
-    <x:t>reply_no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>r_approval</x:t>
-  </x:si>
-  <x:si>
-    <x:t>q_content</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이미지 파일 경로명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>reply_title</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_usestatus</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_required1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>펫 (Pet_tbl)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_explain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>p_gender</x:t>
-  </x:si>
-  <x:si>
-    <x:t>p_unique</x:t>
-  </x:si>
-  <x:si>
-    <x:t>n_content</x:t>
-  </x:si>
-  <x:si>
-    <x:t>admin 고정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>p_picture</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VARCHAR2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>r_status</x:t>
-  </x:si>
-  <x:si>
-    <x:t>s_status</x:t>
-  </x:si>
-  <x:si>
-    <x:t>q_regdate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_optional</x:t>
-  </x:si>
-  <x:si>
-    <x:t>s_explain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>n_regdate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>r_payprice</x:t>
-  </x:si>
-  <x:si>
-    <x:t>p_weight</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c_status</x:t>
-  </x:si>
-  <x:si>
-    <x:t>p_dogbreed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m_required2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>문의 게시판 (QuestionBoard_tbl)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공지사항 (Notice_TBL)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>reply_registrant</x:t>
-  </x:si>
-  <x:si>
-    <x:t>입력값 Y(yes), N(no)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>입력값 unuse, use</x:t>
-  </x:si>
-  <x:si>
-    <x:t>실제 예약 종료날짜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>r_enddate</x:t>
+    <x:t>결제가격</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록일시</x:t>
+  </x:si>
+  <x:si>
+    <x:t>테이블 명세서</x:t>
+  </x:si>
+  <x:si>
+    <x:t>강아지사진</x:t>
+  </x:si>
+  <x:si>
+    <x:t>s_price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>특이사항</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서비스 설명</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1223,6 +1223,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1305,6 +1306,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1339,6 +1341,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1383,6 +1386,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1426,6 +1430,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1510,6 +1515,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1530,6 +1536,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1560,6 +1567,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1812,7 +1820,7 @@
   <x:dimension ref="A1:J266"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="E25" activeCellId="0" sqref="E25:E25"/>
+      <x:selection activeCell="H24" activeCellId="0" sqref="H24:H24"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" customHeight="1"/>
@@ -1841,7 +1849,7 @@
     <x:row r="2" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A2" s="1"/>
       <x:c r="B2" s="28" t="s">
-        <x:v>47</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C2" s="29"/>
       <x:c r="D2" s="29"/>
@@ -1879,7 +1887,7 @@
     <x:row r="5" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A5" s="4"/>
       <x:c r="B5" s="34" t="s">
-        <x:v>55</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C5" s="35"/>
       <x:c r="D5" s="35"/>
@@ -1893,31 +1901,31 @@
     <x:row r="6" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A6" s="4"/>
       <x:c r="B6" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C6" s="11" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D6" s="11" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E6" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F6" s="11" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C6" s="11" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D6" s="11" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E6" s="11" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F6" s="11" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G6" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H6" s="11" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I6" s="11" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="J6" s="11" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10" ht="15.75" customHeight="1">
@@ -1926,28 +1934,28 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C7" s="11" t="s">
-        <x:v>27</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D7" s="11" t="s">
-        <x:v>78</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E7" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F7" s="11">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G7" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H7" s="11" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I7" s="11" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J7" s="11" t="s">
-        <x:v>58</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10" ht="15.75" customHeight="1">
@@ -1956,24 +1964,24 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C8" s="11" t="s">
-        <x:v>10</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="D8" s="11" t="s">
-        <x:v>21</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E8" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F8" s="12">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G8" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H8" s="11"/>
       <x:c r="I8" s="12"/>
       <x:c r="J8" s="11" t="s">
-        <x:v>58</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10" ht="15.75" customHeight="1">
@@ -1982,19 +1990,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C9" s="11" t="s">
-        <x:v>13</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D9" s="11" t="s">
-        <x:v>76</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E9" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F9" s="11">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G9" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H9" s="12"/>
       <x:c r="I9" s="12"/>
@@ -2006,22 +2014,22 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C10" s="11" t="s">
-        <x:v>14</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D10" s="11" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E10" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F10" s="11"/>
       <x:c r="G10" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H10" s="11"/>
       <x:c r="I10" s="12"/>
       <x:c r="J10" s="11" t="s">
-        <x:v>56</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:10" ht="15.75" customHeight="1">
@@ -2030,19 +2038,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C11" s="11" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D11" s="11" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D11" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
       <x:c r="E11" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F11" s="11">
         <x:v>30</x:v>
       </x:c>
       <x:c r="G11" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H11" s="12"/>
       <x:c r="I11" s="12"/>
@@ -2054,24 +2062,24 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C12" s="11" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D12" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E12" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F12" s="11">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G12" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H12" s="12"/>
       <x:c r="I12" s="12"/>
       <x:c r="J12" s="11" t="s">
-        <x:v>52</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" ht="15.75" customHeight="1">
@@ -2080,19 +2088,19 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C13" s="11" t="s">
-        <x:v>94</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D13" s="11" t="s">
-        <x:v>84</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="E13" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F13" s="11">
         <x:v>50</x:v>
       </x:c>
       <x:c r="G13" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H13" s="11"/>
       <x:c r="I13" s="12"/>
@@ -2104,24 +2112,24 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C14" s="11" t="s">
-        <x:v>113</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="D14" s="11" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E14" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F14" s="11">
         <x:v>2</x:v>
       </x:c>
       <x:c r="G14" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H14" s="12"/>
       <x:c r="I14" s="14"/>
       <x:c r="J14" s="15" t="s">
-        <x:v>124</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10" ht="15.75" customHeight="1">
@@ -2130,24 +2138,24 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C15" s="11" t="s">
-        <x:v>101</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D15" s="11" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E15" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F15" s="11">
         <x:v>2</x:v>
       </x:c>
       <x:c r="G15" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H15" s="12"/>
       <x:c r="I15" s="14"/>
       <x:c r="J15" s="15" t="s">
-        <x:v>124</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:10" ht="15.75" customHeight="1">
@@ -2156,24 +2164,24 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C16" s="11" t="s">
-        <x:v>120</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="D16" s="11" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E16" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F16" s="11">
         <x:v>2</x:v>
       </x:c>
       <x:c r="G16" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H16" s="12"/>
       <x:c r="I16" s="14"/>
       <x:c r="J16" s="15" t="s">
-        <x:v>124</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:10" ht="15.75" customHeight="1">
@@ -2191,7 +2199,7 @@
     <x:row r="18" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A18" s="3"/>
       <x:c r="B18" s="34" t="s">
-        <x:v>63</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C18" s="35"/>
       <x:c r="D18" s="35"/>
@@ -2205,25 +2213,25 @@
     <x:row r="19" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A19" s="3"/>
       <x:c r="B19" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C19" s="11" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D19" s="11" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E19" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F19" s="11" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C19" s="11" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D19" s="11" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E19" s="11" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F19" s="11" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G19" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H19" s="11" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I19" s="11" t="s">
         <x:v>71</x:v>
@@ -2236,25 +2244,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C20" s="11" t="s">
-        <x:v>37</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D20" s="11" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E20" s="11" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F20" s="11">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G20" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H20" s="11" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I20" s="11" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J20" s="13"/>
     </x:row>
@@ -2264,24 +2272,24 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C21" s="11" t="s">
-        <x:v>96</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="D21" s="11" t="s">
-        <x:v>2</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E21" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F21" s="12">
         <x:v>2</x:v>
       </x:c>
       <x:c r="G21" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H21" s="11"/>
       <x:c r="I21" s="14"/>
       <x:c r="J21" s="15" t="s">
-        <x:v>124</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:10" ht="15.75" customHeight="1">
@@ -2290,19 +2298,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C22" s="11" t="s">
-        <x:v>116</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="D22" s="11" t="s">
-        <x:v>43</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="E22" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F22" s="11">
         <x:v>7</x:v>
       </x:c>
       <x:c r="G22" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H22" s="12"/>
       <x:c r="I22" s="14"/>
@@ -2314,19 +2322,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C23" s="11" t="s">
-        <x:v>110</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D23" s="11" t="s">
-        <x:v>86</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E23" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F23" s="11">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G23" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H23" s="11"/>
       <x:c r="I23" s="12"/>
@@ -2338,22 +2346,22 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C24" s="11" t="s">
-        <x:v>50</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="D24" s="11" t="s">
         <x:v>25</x:v>
       </x:c>
       <x:c r="E24" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F24" s="11"/>
       <x:c r="G24" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H24" s="12"/>
       <x:c r="I24" s="12"/>
       <x:c r="J24" s="11" t="s">
-        <x:v>56</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:10" ht="15.75" customHeight="1">
@@ -2362,22 +2370,22 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C25" s="11" t="s">
-        <x:v>91</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="D25" s="11" t="s">
-        <x:v>0</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E25" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F25" s="11"/>
       <x:c r="G25" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H25" s="12"/>
       <x:c r="I25" s="12"/>
       <x:c r="J25" s="11" t="s">
-        <x:v>56</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:10" ht="15.75" customHeight="1">
@@ -2386,22 +2394,22 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C26" s="11" t="s">
-        <x:v>127</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="D26" s="11" t="s">
-        <x:v>126</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E26" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F26" s="11"/>
       <x:c r="G26" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H26" s="11"/>
       <x:c r="I26" s="12"/>
       <x:c r="J26" s="11" t="s">
-        <x:v>56</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:10" ht="15.75" customHeight="1">
@@ -2410,23 +2418,23 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C27" s="11" t="s">
-        <x:v>27</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D27" s="11" t="s">
-        <x:v>78</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E27" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F27" s="11">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G27" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H27" s="11"/>
       <x:c r="I27" s="12" t="s">
-        <x:v>72</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="J27" s="11"/>
     </x:row>
@@ -2436,23 +2444,23 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C28" s="11" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D28" s="11" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="D28" s="11" t="s">
-        <x:v>39</x:v>
-      </x:c>
       <x:c r="E28" s="11" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F28" s="11">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G28" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H28" s="12"/>
       <x:c r="I28" s="12" t="s">
-        <x:v>72</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="J28" s="11"/>
     </x:row>
@@ -2471,7 +2479,7 @@
     <x:row r="30" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A30" s="3"/>
       <x:c r="B30" s="37" t="s">
-        <x:v>121</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C30" s="38"/>
       <x:c r="D30" s="38"/>
@@ -2485,25 +2493,25 @@
     <x:row r="31" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A31" s="3"/>
       <x:c r="B31" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C31" s="11" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D31" s="11" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E31" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F31" s="11" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C31" s="11" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D31" s="11" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E31" s="11" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F31" s="11" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G31" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H31" s="11" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I31" s="11" t="s">
         <x:v>71</x:v>
@@ -2516,25 +2524,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C32" s="11" t="s">
-        <x:v>34</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="D32" s="11" t="s">
-        <x:v>85</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E32" s="11" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F32" s="11">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G32" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H32" s="11" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I32" s="11" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J32" s="17"/>
     </x:row>
@@ -2544,19 +2552,19 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C33" s="18" t="s">
-        <x:v>35</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D33" s="11" t="s">
-        <x:v>88</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E33" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F33" s="11">
         <x:v>50</x:v>
       </x:c>
       <x:c r="G33" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H33" s="11"/>
       <x:c r="I33" s="11"/>
@@ -2568,19 +2576,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C34" s="18" t="s">
-        <x:v>97</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="D34" s="11" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E34" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F34" s="11">
         <x:v>3000</x:v>
       </x:c>
       <x:c r="G34" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H34" s="11"/>
       <x:c r="I34" s="11"/>
@@ -2592,22 +2600,22 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C35" s="20" t="s">
-        <x:v>112</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="D35" s="19" t="s">
-        <x:v>46</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="E35" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F35" s="11"/>
       <x:c r="G35" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H35" s="21"/>
       <x:c r="I35" s="21"/>
       <x:c r="J35" s="11" t="s">
-        <x:v>56</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:10" ht="15.75" customHeight="1">
@@ -2616,23 +2624,23 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C36" s="22" t="s">
-        <x:v>27</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D36" s="17" t="s">
-        <x:v>78</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E36" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F36" s="11">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G36" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H36" s="11"/>
       <x:c r="I36" s="23" t="s">
-        <x:v>72</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="J36" s="15"/>
     </x:row>
@@ -2651,7 +2659,7 @@
     <x:row r="38" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A38" s="4"/>
       <x:c r="B38" s="34" t="s">
-        <x:v>122</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C38" s="35"/>
       <x:c r="D38" s="35"/>
@@ -2665,31 +2673,31 @@
     <x:row r="39" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A39" s="6"/>
       <x:c r="B39" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C39" s="11" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D39" s="11" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E39" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F39" s="11" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C39" s="11" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D39" s="11" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E39" s="11" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F39" s="11" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G39" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H39" s="11" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I39" s="11" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="J39" s="11" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:10" ht="15.75" customHeight="1">
@@ -2698,25 +2706,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C40" s="11" t="s">
-        <x:v>40</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D40" s="11" t="s">
-        <x:v>85</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E40" s="11" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F40" s="11">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G40" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H40" s="11" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I40" s="11" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J40" s="11"/>
     </x:row>
@@ -2726,22 +2734,22 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C41" s="11" t="s">
-        <x:v>115</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D41" s="11" t="s">
-        <x:v>46</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="E41" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F41" s="12"/>
       <x:c r="G41" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H41" s="11"/>
       <x:c r="I41" s="12"/>
       <x:c r="J41" s="26" t="s">
-        <x:v>53</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:10" ht="15.75" customHeight="1">
@@ -2750,19 +2758,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C42" s="11" t="s">
-        <x:v>106</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D42" s="11" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E42" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F42" s="11">
         <x:v>3000</x:v>
       </x:c>
       <x:c r="G42" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H42" s="12"/>
       <x:c r="I42" s="12"/>
@@ -2777,16 +2785,16 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="D43" s="11" t="s">
-        <x:v>88</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E43" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F43" s="11">
         <x:v>50</x:v>
       </x:c>
       <x:c r="G43" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H43" s="11"/>
       <x:c r="I43" s="12"/>
@@ -2798,24 +2806,24 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C44" s="11" t="s">
-        <x:v>49</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="D44" s="11" t="s">
-        <x:v>90</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="E44" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F44" s="11">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G44" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H44" s="12"/>
       <x:c r="I44" s="12"/>
       <x:c r="J44" s="11" t="s">
-        <x:v>107</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:10" ht="15.75" customHeight="1">
@@ -2833,7 +2841,7 @@
     <x:row r="46" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A46" s="3"/>
       <x:c r="B46" s="34" t="s">
-        <x:v>60</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C46" s="35"/>
       <x:c r="D46" s="35"/>
@@ -2847,31 +2855,31 @@
     <x:row r="47" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A47" s="4"/>
       <x:c r="B47" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C47" s="11" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D47" s="11" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E47" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F47" s="11" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C47" s="11" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D47" s="11" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E47" s="11" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F47" s="11" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G47" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H47" s="11" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I47" s="11" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="J47" s="11" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:10" ht="15.75" customHeight="1">
@@ -2880,25 +2888,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C48" s="11" t="s">
-        <x:v>36</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D48" s="11" t="s">
-        <x:v>5</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E48" s="11" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F48" s="11">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G48" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H48" s="11" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I48" s="11" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J48" s="11"/>
     </x:row>
@@ -2908,19 +2916,19 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C49" s="11" t="s">
-        <x:v>6</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D49" s="11" t="s">
-        <x:v>64</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E49" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F49" s="12">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G49" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H49" s="11"/>
       <x:c r="I49" s="12"/>
@@ -2932,19 +2940,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C50" s="11" t="s">
-        <x:v>7</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D50" s="11" t="s">
-        <x:v>69</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E50" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F50" s="11">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G50" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H50" s="12"/>
       <x:c r="I50" s="12"/>
@@ -2956,19 +2964,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C51" s="11" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D51" s="11" t="s">
-        <x:v>65</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E51" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F51" s="11">
         <x:v>7</x:v>
       </x:c>
       <x:c r="G51" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H51" s="11"/>
       <x:c r="I51" s="12"/>
@@ -2980,19 +2988,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C52" s="11" t="s">
-        <x:v>103</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="D52" s="11" t="s">
-        <x:v>77</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="E52" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F52" s="11">
         <x:v>1000</x:v>
       </x:c>
       <x:c r="G52" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H52" s="12"/>
       <x:c r="I52" s="12"/>
@@ -3004,24 +3012,24 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C53" s="11" t="s">
-        <x:v>92</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D53" s="11" t="s">
-        <x:v>74</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E53" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F53" s="11">
         <x:v>50</x:v>
       </x:c>
       <x:c r="G53" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H53" s="12"/>
       <x:c r="I53" s="12"/>
       <x:c r="J53" s="17" t="s">
-        <x:v>98</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:10" ht="15.75" customHeight="1">
@@ -3030,24 +3038,24 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C54" s="11" t="s">
-        <x:v>118</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="D54" s="11" t="s">
-        <x:v>86</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E54" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F54" s="11">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G54" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H54" s="11"/>
       <x:c r="I54" s="12"/>
       <x:c r="J54" s="15" t="s">
-        <x:v>125</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:10" ht="15.75" customHeight="1">
@@ -3056,24 +3064,24 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C55" s="11" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="D55" s="11" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E55" s="11" t="s">
         <x:v>100</x:v>
-      </x:c>
-      <x:c r="D55" s="11" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="E55" s="11" t="s">
-        <x:v>109</x:v>
       </x:c>
       <x:c r="F55" s="11">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G55" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H55" s="12"/>
       <x:c r="I55" s="12"/>
       <x:c r="J55" s="15" t="s">
-        <x:v>93</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:10" ht="15.75" customHeight="1">
@@ -3091,7 +3099,7 @@
     <x:row r="57" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A57" s="3"/>
       <x:c r="B57" s="37" t="s">
-        <x:v>102</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C57" s="38"/>
       <x:c r="D57" s="38"/>
@@ -3105,31 +3113,31 @@
     <x:row r="58" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A58" s="3"/>
       <x:c r="B58" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C58" s="11" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D58" s="11" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E58" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F58" s="11" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C58" s="11" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D58" s="11" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E58" s="11" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F58" s="11" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G58" s="11" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H58" s="11" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I58" s="11" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="J58" s="11" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:10" ht="15.75" customHeight="1">
@@ -3138,25 +3146,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C59" s="11" t="s">
-        <x:v>3</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D59" s="11" t="s">
-        <x:v>83</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E59" s="11" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F59" s="11">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G59" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H59" s="11" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I59" s="11" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J59" s="17"/>
     </x:row>
@@ -3166,19 +3174,19 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C60" s="18" t="s">
-        <x:v>8</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D60" s="11" t="s">
-        <x:v>76</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E60" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F60" s="11">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G60" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H60" s="11"/>
       <x:c r="I60" s="11"/>
@@ -3190,19 +3198,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C61" s="18" t="s">
-        <x:v>119</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="D61" s="11" t="s">
-        <x:v>75</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="E61" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F61" s="11">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G61" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H61" s="11"/>
       <x:c r="I61" s="11"/>
@@ -3214,19 +3222,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C62" s="20" t="s">
-        <x:v>105</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="D62" s="19" t="s">
-        <x:v>48</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="E62" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F62" s="11">
         <x:v>200</x:v>
       </x:c>
       <x:c r="G62" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H62" s="21"/>
       <x:c r="I62" s="24"/>
@@ -3238,24 +3246,24 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C63" s="22" t="s">
-        <x:v>104</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="D63" s="17" t="s">
-        <x:v>73</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E63" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F63" s="11">
         <x:v>2</x:v>
       </x:c>
       <x:c r="G63" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H63" s="23"/>
       <x:c r="I63" s="16"/>
       <x:c r="J63" s="15" t="s">
-        <x:v>59</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:10" ht="15.75" customHeight="1">
@@ -3264,24 +3272,24 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C64" s="22" t="s">
-        <x:v>117</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="D64" s="17" t="s">
-        <x:v>89</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="E64" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F64" s="11">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G64" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H64" s="11"/>
       <x:c r="I64" s="23"/>
       <x:c r="J64" s="25" t="s">
-        <x:v>62</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:10" ht="15.75" customHeight="1">
@@ -3290,24 +3298,24 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C65" s="22" t="s">
-        <x:v>108</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D65" s="17" t="s">
-        <x:v>44</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="E65" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F65" s="11">
         <x:v>50</x:v>
       </x:c>
       <x:c r="G65" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H65" s="11"/>
       <x:c r="I65" s="23"/>
       <x:c r="J65" s="17" t="s">
-        <x:v>98</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:10" ht="15.75" customHeight="1">
@@ -3316,23 +3324,23 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C66" s="17" t="s">
-        <x:v>27</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D66" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E66" s="11" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F66" s="11">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G66" s="11" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H66" s="11"/>
       <x:c r="I66" s="23" t="s">
-        <x:v>72</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="J66" s="17"/>
     </x:row>
@@ -3351,7 +3359,7 @@
     <x:row r="68" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A68" s="4"/>
       <x:c r="B68" s="39" t="s">
-        <x:v>61</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C68" s="39"/>
       <x:c r="D68" s="39"/>
@@ -3365,31 +3373,31 @@
     <x:row r="69" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A69" s="4"/>
       <x:c r="B69" s="27" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C69" s="27" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D69" s="27" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E69" s="27" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F69" s="27" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C69" s="27" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D69" s="27" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E69" s="27" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F69" s="27" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G69" s="27" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H69" s="27" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I69" s="27" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="J69" s="16" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:10" ht="15.75" customHeight="1">
@@ -3398,25 +3406,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C70" s="27" t="s">
-        <x:v>23</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D70" s="27" t="s">
-        <x:v>41</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E70" s="27" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F70" s="27">
         <x:v>5</x:v>
       </x:c>
       <x:c r="G70" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H70" s="27" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I70" s="27" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J70" s="16"/>
     </x:row>
@@ -3426,19 +3434,19 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C71" s="27" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D71" s="27" t="s">
-        <x:v>24</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E71" s="27" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F71" s="27">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G71" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H71" s="27"/>
       <x:c r="I71" s="27"/>
@@ -3450,19 +3458,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C72" s="27" t="s">
-        <x:v>114</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="D72" s="27" t="s">
-        <x:v>42</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="E72" s="27" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F72" s="27">
         <x:v>500</x:v>
       </x:c>
       <x:c r="G72" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H72" s="27"/>
       <x:c r="I72" s="27"/>
@@ -3474,24 +3482,24 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C73" s="27" t="s">
-        <x:v>111</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="D73" s="27" t="s">
-        <x:v>86</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E73" s="27" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F73" s="27">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G73" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H73" s="27"/>
       <x:c r="I73" s="27"/>
       <x:c r="J73" s="15" t="s">
-        <x:v>125</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:10" ht="15.75" customHeight="1">
@@ -3500,19 +3508,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C74" s="27" t="s">
-        <x:v>45</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="D74" s="27" t="s">
-        <x:v>65</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E74" s="27" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F74" s="27">
         <x:v>7</x:v>
       </x:c>
       <x:c r="G74" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H74" s="27"/>
       <x:c r="I74" s="27"/>
@@ -3524,23 +3532,23 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C75" s="27" t="s">
-        <x:v>36</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D75" s="27" t="s">
-        <x:v>5</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E75" s="12" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F75" s="11">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G75" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H75" s="27"/>
       <x:c r="I75" s="27" t="s">
-        <x:v>72</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="J75" s="16"/>
     </x:row>
@@ -3559,7 +3567,7 @@
     <x:row r="77" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A77" s="4"/>
       <x:c r="B77" s="39" t="s">
-        <x:v>51</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C77" s="39"/>
       <x:c r="D77" s="39"/>
@@ -3573,31 +3581,31 @@
     <x:row r="78" spans="1:10" ht="15.75" customHeight="1">
       <x:c r="A78" s="4"/>
       <x:c r="B78" s="27" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C78" s="27" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D78" s="27" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E78" s="27" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F78" s="27" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C78" s="27" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="D78" s="27" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="E78" s="27" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F78" s="27" t="s">
-        <x:v>79</x:v>
-      </x:c>
       <x:c r="G78" s="27" t="s">
-        <x:v>19</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H78" s="27" t="s">
-        <x:v>87</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I78" s="27" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="J78" s="16" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:10" ht="15.75" customHeight="1">
@@ -3606,25 +3614,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C79" s="27" t="s">
-        <x:v>95</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="D79" s="27" t="s">
-        <x:v>38</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E79" s="27" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F79" s="27">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G79" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H79" s="27" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I79" s="27" t="s">
-        <x:v>81</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J79" s="16"/>
     </x:row>
@@ -3634,24 +3642,24 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C80" s="27" t="s">
-        <x:v>54</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="D80" s="27" t="s">
-        <x:v>46</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="E80" s="27" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F80" s="27" t="s">
-        <x:v>22</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G80" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H80" s="27"/>
       <x:c r="I80" s="27"/>
       <x:c r="J80" s="11" t="s">
-        <x:v>56</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:10" ht="15.75" customHeight="1">
@@ -3660,19 +3668,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C81" s="27" t="s">
-        <x:v>57</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="D81" s="27" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E81" s="27" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F81" s="27">
         <x:v>1000</x:v>
       </x:c>
       <x:c r="G81" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H81" s="27"/>
       <x:c r="I81" s="27"/>
@@ -3684,19 +3692,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C82" s="27" t="s">
-        <x:v>99</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D82" s="27" t="s">
-        <x:v>88</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E82" s="27" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F82" s="27">
         <x:v>50</x:v>
       </x:c>
       <x:c r="G82" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H82" s="27"/>
       <x:c r="I82" s="27"/>
@@ -3708,19 +3716,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C83" s="27" t="s">
-        <x:v>123</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="D83" s="27" t="s">
-        <x:v>90</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="E83" s="27" t="s">
-        <x:v>109</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F83" s="27">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G83" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H83" s="27"/>
       <x:c r="I83" s="27"/>
@@ -3732,25 +3740,25 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C84" s="27" t="s">
-        <x:v>34</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="D84" s="27" t="s">
-        <x:v>85</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E84" s="27" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F84" s="27">
         <x:v>6</x:v>
       </x:c>
       <x:c r="G84" s="27" t="s">
-        <x:v>66</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H84" s="27" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="I84" s="27" t="s">
-        <x:v>72</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="J84" s="16"/>
     </x:row>

</xml_diff>